<commit_message>
Service info for game statistics
</commit_message>
<xml_diff>
--- a/_work/Statistik.xlsx
+++ b/_work/Statistik.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="83">
   <si>
     <t>Lea</t>
   </si>
@@ -167,6 +167,105 @@
   </si>
   <si>
     <t>21:23:w:Nadine/Magda</t>
+  </si>
+  <si>
+    <t>1:s:Celi</t>
+  </si>
+  <si>
+    <t>2:s:Therry</t>
+  </si>
+  <si>
+    <t>4:s:Nadine</t>
+  </si>
+  <si>
+    <t>6:s:Nina</t>
+  </si>
+  <si>
+    <t>7:s:Lea</t>
+  </si>
+  <si>
+    <t>13:s:Kati</t>
+  </si>
+  <si>
+    <t>20:s:Celi</t>
+  </si>
+  <si>
+    <t>0:s:Celi</t>
+  </si>
+  <si>
+    <t>2:s:Nadine</t>
+  </si>
+  <si>
+    <t>4:s:Nina</t>
+  </si>
+  <si>
+    <t>12:s:Katha</t>
+  </si>
+  <si>
+    <t>14:s:Celi</t>
+  </si>
+  <si>
+    <t>15:s:Therry</t>
+  </si>
+  <si>
+    <t>16:s:Nadine</t>
+  </si>
+  <si>
+    <t>19:s:Nina</t>
+  </si>
+  <si>
+    <t>20:s:Lea</t>
+  </si>
+  <si>
+    <t>5:s:Therry</t>
+  </si>
+  <si>
+    <t>7:s:Nadine</t>
+  </si>
+  <si>
+    <t>10:s:Nina</t>
+  </si>
+  <si>
+    <t>14:s:Lea</t>
+  </si>
+  <si>
+    <t>15:s:Kati</t>
+  </si>
+  <si>
+    <t>16:s:Celi</t>
+  </si>
+  <si>
+    <t>18:s:Nadine</t>
+  </si>
+  <si>
+    <t>20:s:Nina</t>
+  </si>
+  <si>
+    <t>22:s:Lea</t>
+  </si>
+  <si>
+    <t>9:s:Therry</t>
+  </si>
+  <si>
+    <t>13:s:Nadine</t>
+  </si>
+  <si>
+    <t>14:s:Nina</t>
+  </si>
+  <si>
+    <t>15:s:Lea</t>
+  </si>
+  <si>
+    <t>16:s:Kati</t>
+  </si>
+  <si>
+    <t>21:s:Therry</t>
+  </si>
+  <si>
+    <t>24:s:Lea</t>
+  </si>
+  <si>
+    <t>23:s:Magda</t>
   </si>
 </sst>
 </file>
@@ -730,7 +829,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AF23" sqref="AF23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -964,16 +1065,16 @@
         <v>8</v>
       </c>
       <c r="AC10" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="AD10" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="AE10" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="AF10" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
@@ -1049,16 +1150,16 @@
         <v>12</v>
       </c>
       <c r="AC11" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="AD11" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="AE11" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="AF11" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.25">
@@ -1134,13 +1235,16 @@
         <v>13</v>
       </c>
       <c r="AC12" t="s">
-        <v>36</v>
+        <v>52</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>59</v>
       </c>
       <c r="AE12" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="AF12" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
@@ -1215,11 +1319,17 @@
       <c r="Z13">
         <v>14</v>
       </c>
+      <c r="AC13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>54</v>
+      </c>
       <c r="AE13" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="AF13" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.25">
@@ -1282,11 +1392,17 @@
       <c r="Z14">
         <v>15</v>
       </c>
+      <c r="AC14" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>60</v>
+      </c>
       <c r="AE14" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="AF14" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.25">
@@ -1349,8 +1465,17 @@
       <c r="Z15">
         <v>19</v>
       </c>
+      <c r="AC15" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>40</v>
+      </c>
       <c r="AF15" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.25">
@@ -1425,8 +1550,20 @@
       <c r="Z16">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AC16" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
@@ -1495,8 +1632,20 @@
       <c r="Z17">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AC17" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4">
         <v>25</v>
@@ -1559,8 +1708,20 @@
       <c r="Z18">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AC18" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>71</v>
+      </c>
+      <c r="AF18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="U19">
         <v>14</v>
       </c>
@@ -1579,8 +1740,20 @@
       <c r="Z19">
         <v>23</v>
       </c>
-    </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AC19" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>72</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1602,8 +1775,17 @@
       <c r="Z20">
         <v>25</v>
       </c>
-    </row>
-    <row r="21" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AD20" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:32" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="8">
         <v>43404</v>
       </c>
@@ -1630,8 +1812,17 @@
       <c r="X21">
         <v>22</v>
       </c>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AD21" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4" t="s">
         <v>15</v>
@@ -1660,8 +1851,14 @@
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
       <c r="P22" s="6"/>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AE22" t="s">
+        <v>73</v>
+      </c>
+      <c r="AF22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="7" t="s">
         <v>13</v>
@@ -1706,8 +1903,14 @@
       <c r="P23" s="6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AE23" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4">
         <v>25</v>
@@ -1748,8 +1951,19 @@
         <f t="shared" ref="P24" si="16" xml:space="preserve"> IF(M24+N24=0, 0, IF(N24=0, "MAX", M24/N24))</f>
         <v>1.5</v>
       </c>
-    </row>
-    <row r="26" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AE24" t="s">
+        <v>74</v>
+      </c>
+      <c r="AF24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AF25" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:32" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="8">
         <v>43399</v>
       </c>
@@ -1771,7 +1985,7 @@
       <c r="O26" s="9"/>
       <c r="P26" s="10"/>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4" t="s">
         <v>15</v>
@@ -1801,7 +2015,7 @@
       <c r="O27" s="4"/>
       <c r="P27" s="6"/>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="7" t="s">
         <v>13</v>
@@ -1862,7 +2076,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>8</v>
       </c>
@@ -1914,7 +2128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>2</v>
       </c>
@@ -1975,7 +2189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>3</v>
       </c>
@@ -2030,7 +2244,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
updated match statistics (4.11.)
</commit_message>
<xml_diff>
--- a/_work/Statistik.xlsx
+++ b/_work/Statistik.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="84">
   <si>
     <t>Lea</t>
   </si>
@@ -266,6 +266,9 @@
   </si>
   <si>
     <t>23:s:Magda</t>
+  </si>
+  <si>
+    <t>17:s:Therry</t>
   </si>
 </sst>
 </file>
@@ -830,7 +833,7 @@
   <dimension ref="A1:AG73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AF23" sqref="AF23"/>
+      <selection activeCell="AE20" sqref="AE20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1747,7 +1750,7 @@
         <v>64</v>
       </c>
       <c r="AE19" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="AF19" t="s">
         <v>80</v>
@@ -1779,7 +1782,7 @@
         <v>65</v>
       </c>
       <c r="AE20" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="AF20" t="s">
         <v>46</v>
@@ -1816,7 +1819,7 @@
         <v>38</v>
       </c>
       <c r="AE21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AF21" t="s">
         <v>47</v>
@@ -1852,7 +1855,7 @@
       <c r="O22" s="4"/>
       <c r="P22" s="6"/>
       <c r="AE22" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="AF22" t="s">
         <v>82</v>
@@ -1904,7 +1907,7 @@
         <v>22</v>
       </c>
       <c r="AE23" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="AF23" t="s">
         <v>48</v>
@@ -1952,13 +1955,16 @@
         <v>1.5</v>
       </c>
       <c r="AE24" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="AF24" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AE25" t="s">
+        <v>74</v>
+      </c>
       <c r="AF25" t="s">
         <v>81</v>
       </c>

</xml_diff>

<commit_message>
statistics - error correction
</commit_message>
<xml_diff>
--- a/_work/Statistik.xlsx
+++ b/_work/Statistik.xlsx
@@ -1398,7 +1398,7 @@
   <dimension ref="A1:AM142"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1931,7 +1931,7 @@
         <v>0</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -1944,7 +1944,7 @@
       </c>
       <c r="M9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N9">
         <f t="shared" si="1"/>
@@ -1952,14 +1952,15 @@
       </c>
       <c r="O9" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P9" s="3">
+        <v>1</v>
+      </c>
+      <c r="P9" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>MAX</v>
       </c>
       <c r="Q9">
-        <v>2</v>
+        <f>IF(P9 &lt; 1, 3, IF(P9 &gt;= P$17, 1, 2))</f>
+        <v>1</v>
       </c>
       <c r="S9">
         <v>12</v>

</xml_diff>